<commit_message>
Added rule about notification in case of data delivery is not on the computational grid (V1.5).
</commit_message>
<xml_diff>
--- a/esgf_data_submission/forms/CORDEX_ESGF_data_submission_form.xlsx
+++ b/esgf_data_submission/forms/CORDEX_ESGF_data_submission_form.xlsx
@@ -44,10 +44,10 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Heinz-Dieter Hollweg - Persönliche Ansicht" guid="{FF4C21BB-01EC-4FF2-8909-E522D2CCA860}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" tabRatio="214" activeSheetId="1"/>
+    <customWorkbookView name="Karin Meier-Fleischer - Persönliche Ansicht" guid="{3C9A1B9A-18C0-485E-B0F5-D3BF50A001C5}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1818" windowHeight="861" tabRatio="214" activeSheetId="1"/>
+    <customWorkbookView name="Ole B Christensen - Privat visning" guid="{066293A7-3B6A-4B4E-989A-3AE9C9693149}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1676" windowHeight="908" tabRatio="214" activeSheetId="1" showComments="commIndAndComment"/>
     <customWorkbookView name="Stephanie Legutke - Persönliche Ansicht" guid="{4D093F72-1DF5-4965-BD9A-E1DB76A854CB}" autoUpdate="1" mergeInterval="10" personalView="1" maximized="1" windowWidth="1690" windowHeight="873" tabRatio="256" activeSheetId="1" showComments="commIndAndComment"/>
-    <customWorkbookView name="Ole B Christensen - Privat visning" guid="{066293A7-3B6A-4B4E-989A-3AE9C9693149}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1676" windowHeight="908" tabRatio="214" activeSheetId="1" showComments="commIndAndComment"/>
-    <customWorkbookView name="Karin Meier-Fleischer - Persönliche Ansicht" guid="{3C9A1B9A-18C0-485E-B0F5-D3BF50A001C5}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1818" windowHeight="861" tabRatio="214" activeSheetId="1"/>
-    <customWorkbookView name="Heinz-Dieter Hollweg - Persönliche Ansicht" guid="{FF4C21BB-01EC-4FF2-8909-E522D2CCA860}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" tabRatio="214" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -554,6 +554,208 @@
     <t>Give the CORDEX domain identifier of your data. These are composed of a region identifier and a resolution identifier separated by a dash. It has to equal the value of the global NetCDF attribute 'CORDEX_domain' in the files.</t>
   </si>
   <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>institute_id</t>
+  </si>
+  <si>
+    <t>institution</t>
+  </si>
+  <si>
+    <t>model_id</t>
+  </si>
+  <si>
+    <t>experiment_id</t>
+  </si>
+  <si>
+    <t>rcm_version_id</t>
+  </si>
+  <si>
+    <t>grid_mapping_name</t>
+  </si>
+  <si>
+    <t>CORDEX_domain</t>
+  </si>
+  <si>
+    <t>grid_as_specified_if_rotated_pole</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>terms_of_use</t>
+  </si>
+  <si>
+    <t>directory_structure</t>
+  </si>
+  <si>
+    <t>data_path</t>
+  </si>
+  <si>
+    <t>exclude_variables_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uniqueness of tracking_id and creation_date                                                         </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://verc.enes.org/data/projects/documents/cordex-archive-design</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Not Applicable</t>
+    </r>
+  </si>
+  <si>
+    <t>provided ?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Please update the date in field C4 of sheet 'General info'. The date will be transfered to the other sheets.</t>
+  </si>
+  <si>
+    <t>Please do not delete any row in the frequency sheets. Just mark the variables you are not going to submit with 'no'. Please do this for ALL frequency sheets.</t>
+  </si>
+  <si>
+    <t>Version:</t>
+  </si>
+  <si>
+    <r>
+      <t>The value of this field has to equal the value of the global NetCDF attribute 'institute_id' in the data files and must equal the 4th directory level. It is needed before the publication process is started in order that the value can be added to the relevant CORDEX list of CV</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> if not yet there. Note that 'institute_id' has to be the first part of 'model_id'.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The value of this field has to be the value of the global NetCDF attribute 'model_id' in the data files. It is needed before the publication process is started in order that the value can be added to the relevant CORDEX list of CV</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> if not yet there. Note that it must be composed by the 'institute_id' follwed by the RCM CORDEX model name, separated by a dash. It is part of the file name and the directory structure.</t>
+    </r>
+  </si>
+  <si>
+    <t>The value of this field must equal the respective CMIP5 experiment member of the forcing data and the value of the NetCDF attribute 'driving_model_ensemble_member'. It is part of the file name and the directory structure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The value of this field has to equal that of the globalNetCDF attribute 'rcm_version_id' in the data files.  It is part of the file name and the directory structure. Please give the full string between the underscores. </t>
+  </si>
+  <si>
+    <t>Give the NetCDF/CF name of the data grid ('rotated_latitude_longitude', 'lambert_conformal_conic', etc.), i.e. either that of the native model grid, or 'latitude_longitude' for the regular -XXi grids.</t>
+  </si>
+  <si>
+    <r>
+      <t>In each CORDEX file there may be only one variable which shall be published and searchable at the ESGF portal (target variable). In order to facilitate publication, all non-target variables are included in a list used by the publisher to avoid publication. A list of known non-target variables is [time, time_bnds, lon, lat, rlon ,rlat ,x ,y ,z ,height, plev, Lambert_Conformal, rotated_pole]. Please enter other variables into the left field if applicable (e.g. grid description variables), otherwise write 'N/A'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>The value of this field has to equal the value of the optional NetCDF attribute 'institution' (long version) in the data files if the latter is used.</t>
+  </si>
+  <si>
+    <t>hurs</t>
+  </si>
+  <si>
+    <t>Note: The hurs  variable has been added later to the list and may be omitted</t>
+  </si>
+  <si>
+    <t>driving_model_id</t>
+  </si>
+  <si>
+    <t>Please note that data with file names or directory structure that deviate from those below may be rejected.</t>
+  </si>
+  <si>
+    <t>This form contains one sheet for each frequency for which Tier1 or Core data is requested corresponding to the 'data requirements' excel spread sheet.
+We ask you to mark the variables, for which you request publication in the CORDEX ESGF archive. The method to do that has been changed in order to allow automated processing of the spread sheet content. 
+Now there are 4 values allowed in the field of column 'B' next to the variable name:
+- 'no' if the variable will not be provided with the present request for publication 
+- 'yes' if the variable will be provided  with the present request for publication (default already in the fields)
+- 'un-publish' if data, already published in the ESGF, shall be unpublished
+- 're-publish' if data shall be unpublished and a new version is provided with the present request that shall be published
+The values for variables which are already published and shall stay in the ESGF, have to remain untouched.
+In case data has to be un-published ('re-publish' or 'un-publish') the ESGF version number of the data to be unpublished has to be given in the field of column 'C' next to the variable. It is found in the 'Results' tag on the search page (Version: ...) in the ESGF portal.
+In addition, a short note about the causes for the un-publish (or re-publish) request has to be given. This text will be included on the 'Errata' page 'CORDEX@DKRZ' at the ESGF portal entry page of DKRZ (esgf-data.dkrz.de).
+The filled-in submission sheet should then always reflect the actual state
+It is recommended to use a single form for a single experiment and for a single domain. All variables of a specific experiment have to be provided for the same period. Other periods may be given exceptionally in the frequency sheets in column 'Comments by the data provider'.</t>
+  </si>
+  <si>
     <r>
       <t>Does the grid configuration exactly follow the specifications in ADD</t>
     </r>
@@ -589,213 +791,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>.</t>
+      <t>. If the data is not delivered on the computational grid it has to be noted here as well.</t>
     </r>
   </si>
   <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>institute_id</t>
-  </si>
-  <si>
-    <t>institution</t>
-  </si>
-  <si>
-    <t>model_id</t>
-  </si>
-  <si>
-    <t>experiment_id</t>
-  </si>
-  <si>
-    <t>rcm_version_id</t>
-  </si>
-  <si>
-    <t>grid_mapping_name</t>
-  </si>
-  <si>
-    <t>CORDEX_domain</t>
-  </si>
-  <si>
-    <t>grid_as_specified_if_rotated_pole</t>
-  </si>
-  <si>
-    <t>QC</t>
-  </si>
-  <si>
-    <t>terms_of_use</t>
-  </si>
-  <si>
-    <t>directory_structure</t>
-  </si>
-  <si>
-    <t>data_path</t>
-  </si>
-  <si>
-    <t>exclude_variables_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uniqueness of tracking_id and creation_date                                                         </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> https://verc.enes.org/data/projects/documents/cordex-archive-design</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Not Applicable</t>
-    </r>
-  </si>
-  <si>
-    <t>provided ?</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Please update the date in field C4 of sheet 'General info'. The date will be transfered to the other sheets.</t>
-  </si>
-  <si>
-    <t>Please do not delete any row in the frequency sheets. Just mark the variables you are not going to submit with 'no'. Please do this for ALL frequency sheets.</t>
-  </si>
-  <si>
-    <t>Version:</t>
-  </si>
-  <si>
-    <r>
-      <t>The value of this field has to equal the value of the global NetCDF attribute 'institute_id' in the data files and must equal the 4th directory level. It is needed before the publication process is started in order that the value can be added to the relevant CORDEX list of CV</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> if not yet there. Note that 'institute_id' has to be the first part of 'model_id'.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>The value of this field has to be the value of the global NetCDF attribute 'model_id' in the data files. It is needed before the publication process is started in order that the value can be added to the relevant CORDEX list of CV</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> if not yet there. Note that it must be composed by the 'institute_id' follwed by the RCM CORDEX model name, separated by a dash. It is part of the file name and the directory structure.</t>
-    </r>
-  </si>
-  <si>
-    <t>The value of this field must equal the respective CMIP5 experiment member of the forcing data and the value of the NetCDF attribute 'driving_model_ensemble_member'. It is part of the file name and the directory structure.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The value of this field has to equal that of the globalNetCDF attribute 'rcm_version_id' in the data files.  It is part of the file name and the directory structure. Please give the full string between the underscores. </t>
-  </si>
-  <si>
-    <t>Give the NetCDF/CF name of the data grid ('rotated_latitude_longitude', 'lambert_conformal_conic', etc.), i.e. either that of the native model grid, or 'latitude_longitude' for the regular -XXi grids.</t>
-  </si>
-  <si>
-    <r>
-      <t>In each CORDEX file there may be only one variable which shall be published and searchable at the ESGF portal (target variable). In order to facilitate publication, all non-target variables are included in a list used by the publisher to avoid publication. A list of known non-target variables is [time, time_bnds, lon, lat, rlon ,rlat ,x ,y ,z ,height, plev, Lambert_Conformal, rotated_pole]. Please enter other variables into the left field if applicable (e.g. grid description variables), otherwise write 'N/A'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>The value of this field has to equal the value of the optional NetCDF attribute 'institution' (long version) in the data files if the latter is used.</t>
-  </si>
-  <si>
-    <t>hurs</t>
-  </si>
-  <si>
-    <t>Note: The hurs  variable has been added later to the list and may be omitted</t>
-  </si>
-  <si>
-    <t>driving_model_id</t>
-  </si>
-  <si>
-    <t>Please note that data with file names or directory structure that deviate from those below may be rejected.</t>
-  </si>
-  <si>
-    <t>This form contains one sheet for each frequency for which Tier1 or Core data is requested corresponding to the 'data requirements' excel spread sheet.
-We ask you to mark the variables, for which you request publication in the CORDEX ESGF archive. The method to do that has been changed in order to allow automated processing of the spread sheet content. 
-Now there are 4 values allowed in the field of column 'B' next to the variable name:
-- 'no' if the variable will not be provided with the present request for publication 
-- 'yes' if the variable will be provided  with the present request for publication (default already in the fields)
-- 'un-publish' if data, already published in the ESGF, shall be unpublished
-- 're-publish' if data shall be unpublished and a new version is provided with the present request that shall be published
-The values for variables which are already published and shall stay in the ESGF, have to remain untouched.
-In case data has to be un-published ('re-publish' or 'un-publish') the ESGF version number of the data to be unpublished has to be given in the field of column 'C' next to the variable. It is found in the 'Results' tag on the search page (Version: ...) in the ESGF portal.
-In addition, a short note about the causes for the un-publish (or re-publish) request has to be given. This text will be included on the 'Errata' page 'CORDEX@DKRZ' at the ESGF portal entry page of DKRZ (esgf-data.dkrz.de).
-The filled-in submission sheet should then always reflect the actual state
-It is recommended to use a single form for a single experiment and for a single domain. All variables of a specific experiment have to be provided for the same period. Other periods may be given exceptionally in the frequency sheets in column 'Comments by the data provider'.</t>
-  </si>
-  <si>
-    <t>V1.4</t>
+    <t>V1.5</t>
   </si>
 </sst>
 </file>
@@ -1698,23 +1698,74 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1761,59 +1812,8 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2337,7 +2337,7 @@
     </row>
     <row r="2" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C2" s="43" t="s">
         <v>144</v>
@@ -2348,11 +2348,11 @@
     </row>
     <row r="3" spans="1:7" s="13" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
     </row>
     <row r="4" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
@@ -2382,79 +2382,79 @@
     </row>
     <row r="7" spans="1:7" ht="237.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
-      <c r="B7" s="77" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
+      <c r="B7" s="81" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="79" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" s="79"/>
+      <c r="C11" s="78" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="78"/>
     </row>
     <row r="12" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="79" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="79"/>
+      <c r="C12" s="78" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="78"/>
     </row>
     <row r="13" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="79"/>
+      <c r="D13" s="78"/>
     </row>
     <row r="14" spans="1:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="81" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
+      <c r="B14" s="79" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
     </row>
     <row r="15" spans="1:7" s="35" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="80" t="s">
+      <c r="C15" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="80"/>
+      <c r="D15" s="77"/>
       <c r="E15" s="38"/>
       <c r="F15" s="38"/>
       <c r="G15" s="38"/>
@@ -2474,10 +2474,10 @@
       <c r="B17" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="80" t="s">
+      <c r="C17" s="77" t="s">
         <v>96</v>
       </c>
-      <c r="D17" s="80"/>
+      <c r="D17" s="77"/>
       <c r="E17" s="38"/>
       <c r="F17" s="38"/>
       <c r="G17" s="38"/>
@@ -2570,17 +2570,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B10:D10"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.39370078740157483"/>
@@ -2593,8 +2593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:G26"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2618,10 +2618,10 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:10" s="12" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="100" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="84"/>
+      <c r="B2" s="101"/>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
@@ -2629,14 +2629,14 @@
       <c r="G2" s="28"/>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="94" t="s">
+      <c r="B3" s="112"/>
+      <c r="C3" s="111" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="95"/>
+      <c r="D3" s="112"/>
       <c r="E3" s="24" t="s">
         <v>83</v>
       </c>
@@ -2648,12 +2648,12 @@
       </c>
     </row>
     <row r="4" spans="1:10" s="12" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="97"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="114"/>
       <c r="E4" s="42" t="s">
         <v>104</v>
       </c>
@@ -2661,12 +2661,12 @@
       <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:10" s="12" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="86" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="93"/>
+      <c r="A5" s="103" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="104"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="110"/>
       <c r="E5" s="31" t="s">
         <v>105</v>
       </c>
@@ -2674,47 +2674,47 @@
       <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:10" s="12" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="91"/>
+      <c r="A6" s="105" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="106"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="108"/>
       <c r="E6" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:10" s="12" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A7" s="88" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="91"/>
+      <c r="A7" s="105" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="106"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="108"/>
       <c r="E7" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:10" s="12" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.25">
-      <c r="A8" s="88" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="91"/>
+      <c r="A8" s="105" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="106"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="108"/>
       <c r="E8" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:10" s="12" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A9" s="66" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>98</v>
@@ -2728,12 +2728,12 @@
       <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:10" s="12" customFormat="1" ht="81.599999999999994" x14ac:dyDescent="0.25">
-      <c r="A10" s="98" t="s">
-        <v>141</v>
-      </c>
-      <c r="B10" s="99"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="102"/>
+      <c r="A10" s="95" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="96"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="97"/>
       <c r="E10" s="23" t="s">
         <v>107</v>
       </c>
@@ -2742,78 +2742,78 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" s="12" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="98" t="s">
+      <c r="A11" s="95" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="99"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="102"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="97"/>
       <c r="E11" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F11" s="50"/>
       <c r="G11" s="23"/>
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" s="12" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="98" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="99"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="102"/>
+      <c r="A12" s="95" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="96"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="97"/>
       <c r="E12" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:10" s="12" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="98" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="99"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="102"/>
+      <c r="A13" s="95" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="96"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="97"/>
       <c r="E13" s="45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:10" s="12" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="98" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="99"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="101"/>
+      <c r="A14" s="95" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="96"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="88"/>
       <c r="E14" s="23" t="s">
         <v>108</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
     </row>
-    <row r="15" spans="1:10" ht="44.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="103" t="s">
-        <v>118</v>
-      </c>
-      <c r="B15" s="104"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="106"/>
+    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="86"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="99"/>
       <c r="E15" s="23" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="F15" s="49"/>
       <c r="G15" s="51"/>
     </row>
     <row r="16" spans="1:10" s="12" customFormat="1" ht="59.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="103" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="104"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="101"/>
+      <c r="A16" s="85" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="86"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="88"/>
       <c r="E16" s="23" t="s">
         <v>103</v>
       </c>
@@ -2821,12 +2821,12 @@
       <c r="G16" s="23"/>
     </row>
     <row r="17" spans="1:7" s="12" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="103" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="100"/>
-      <c r="D17" s="101"/>
+      <c r="A17" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="86"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="88"/>
       <c r="E17" s="23" t="s">
         <v>101</v>
       </c>
@@ -2834,12 +2834,12 @@
       <c r="G17" s="23"/>
     </row>
     <row r="18" spans="1:7" s="12" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="103" t="s">
-        <v>121</v>
-      </c>
-      <c r="B18" s="104"/>
-      <c r="C18" s="100"/>
-      <c r="D18" s="101"/>
+      <c r="A18" s="85" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="86"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="88"/>
       <c r="E18" s="23" t="s">
         <v>99</v>
       </c>
@@ -2847,12 +2847,12 @@
       <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="103" t="s">
-        <v>122</v>
-      </c>
-      <c r="B19" s="104"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="101"/>
+      <c r="A19" s="85" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="86"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="88"/>
       <c r="E19" s="23" t="s">
         <v>102</v>
       </c>
@@ -2860,25 +2860,25 @@
       <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7" s="12" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="103" t="s">
-        <v>123</v>
-      </c>
-      <c r="B20" s="104"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="101"/>
+      <c r="A20" s="85" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="86"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="88"/>
       <c r="E20" s="44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F20" s="41"/>
       <c r="G20" s="41"/>
     </row>
     <row r="21" spans="1:7" s="12" customFormat="1" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="109" t="s">
-        <v>124</v>
-      </c>
-      <c r="B21" s="110"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="112"/>
+      <c r="A21" s="90" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="91"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="93"/>
       <c r="E21" s="29" t="s">
         <v>100</v>
       </c>
@@ -2886,10 +2886,10 @@
       <c r="G21" s="29"/>
     </row>
     <row r="22" spans="1:7" s="12" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="113" t="s">
+      <c r="A22" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="113"/>
+      <c r="B22" s="94"/>
       <c r="C22" s="40"/>
       <c r="D22" s="40"/>
       <c r="E22" s="40"/>
@@ -2897,41 +2897,41 @@
       <c r="G22" s="13"/>
     </row>
     <row r="23" spans="1:7" s="12" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="108" t="s">
+      <c r="A23" s="89" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="89"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+    </row>
+    <row r="24" spans="1:7" s="12" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="89" t="s">
         <v>125</v>
       </c>
-      <c r="B23" s="108"/>
-      <c r="C23" s="108"/>
-      <c r="D23" s="108"/>
-      <c r="E23" s="108"/>
-    </row>
-    <row r="24" spans="1:7" s="12" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="108" t="s">
-        <v>126</v>
-      </c>
-      <c r="B24" s="108"/>
-      <c r="C24" s="108"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
       <c r="D24" s="46"/>
       <c r="E24" s="46"/>
     </row>
     <row r="25" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="107" t="str">
+      <c r="A25" s="84" t="str">
         <f>IF(OR(ISBLANK(C4),ISBLANK(C5),ISBLANK(C6),ISBLANK(C8),ISBLANK(C9),ISBLANK(D9),ISBLANK(C10),ISBLANK(C11),ISBLANK(C12),ISBLANK(C13),ISBLANK(C14),ISBLANK(C16),ISBLANK(C17),ISBLANK(C18),ISBLANK(C19),AND(NOT(EXACT(C21,"yes")),NOT(EXACT(C21,"N/A")))),"Not yet complete or correct. Please fill in all fields!","Now check DRS file name and directory structure in sheet 'ReadMe'")</f>
         <v>Not yet complete or correct. Please fill in all fields!</v>
       </c>
-      <c r="B25" s="107"/>
-      <c r="C25" s="107"/>
-      <c r="D25" s="107"/>
-      <c r="E25" s="107"/>
+      <c r="B25" s="84"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
     </row>
     <row r="26" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="115"/>
-      <c r="B26" s="115"/>
-      <c r="C26" s="115"/>
-      <c r="D26" s="115"/>
-      <c r="E26" s="115"/>
-      <c r="F26" s="115"/>
-      <c r="G26" s="115"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="83"/>
     </row>
     <row r="27" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2942,6 +2942,33 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A18:B18"/>
@@ -2957,33 +2984,6 @@
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="A26">
     <cfRule type="containsText" dxfId="15" priority="2" stopIfTrue="1" operator="containsText" text="&quot;Now check DRS file name and directory structure in sheet 'ReadMe'&quot;">
@@ -3057,7 +3057,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>78</v>
@@ -3074,7 +3074,7 @@
         <v>57</v>
       </c>
       <c r="B4" s="76" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="55"/>
       <c r="D4" s="73" t="str">
@@ -3090,7 +3090,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="60" t="str">
@@ -3106,7 +3106,7 @@
         <v>59</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="60" t="str">
@@ -3122,7 +3122,7 @@
         <v>58</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="60" t="str">
@@ -3138,7 +3138,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="74" t="str">
@@ -3154,7 +3154,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="59"/>
       <c r="D9" s="60" t="str">
@@ -3170,7 +3170,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="75" t="str">
@@ -3186,7 +3186,7 @@
         <v>60</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="60" t="str">
@@ -3202,7 +3202,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="60" t="str">
@@ -3218,7 +3218,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="60" t="str">
@@ -3231,10 +3231,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B14" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="60" t="str">
@@ -3250,7 +3250,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="60" t="str">
@@ -3266,7 +3266,7 @@
         <v>41</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C16" s="59"/>
       <c r="D16" s="60" t="str">
@@ -3282,7 +3282,7 @@
         <v>65</v>
       </c>
       <c r="B17" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="60" t="str">
@@ -3298,7 +3298,7 @@
         <v>53</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="60" t="str">
@@ -3314,7 +3314,7 @@
         <v>52</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" s="59"/>
       <c r="D19" s="60" t="str">
@@ -3330,7 +3330,7 @@
         <v>54</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" s="59"/>
       <c r="D20" s="60" t="str">
@@ -3346,7 +3346,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="60" t="str">
@@ -3362,7 +3362,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="59"/>
       <c r="D22" s="60" t="str">
@@ -3378,7 +3378,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C23" s="59"/>
       <c r="D23" s="60" t="str">
@@ -3394,7 +3394,7 @@
         <v>62</v>
       </c>
       <c r="B24" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C24" s="68"/>
       <c r="D24" s="69" t="str">
@@ -3410,7 +3410,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C25" s="59"/>
       <c r="D25" s="60" t="str">
@@ -3426,7 +3426,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="59"/>
       <c r="D26" s="60" t="str">
@@ -3442,7 +3442,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C27" s="59"/>
       <c r="D27" s="60" t="str">
@@ -3458,7 +3458,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C28" s="59"/>
       <c r="D28" s="60" t="str">
@@ -3474,7 +3474,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" s="59"/>
       <c r="D29" s="60" t="str">
@@ -3490,7 +3490,7 @@
         <v>21</v>
       </c>
       <c r="B30" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C30" s="59"/>
       <c r="D30" s="60" t="str">
@@ -3506,7 +3506,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C31" s="59"/>
       <c r="D31" s="60" t="str">
@@ -3522,7 +3522,7 @@
         <v>22</v>
       </c>
       <c r="B32" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C32" s="59"/>
       <c r="D32" s="60" t="str">
@@ -3538,7 +3538,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C33" s="59"/>
       <c r="D33" s="60" t="str">
@@ -3554,7 +3554,7 @@
         <v>23</v>
       </c>
       <c r="B34" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C34" s="59"/>
       <c r="D34" s="60" t="str">
@@ -3570,7 +3570,7 @@
         <v>63</v>
       </c>
       <c r="B35" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" s="59"/>
       <c r="D35" s="60" t="str">
@@ -3586,7 +3586,7 @@
         <v>64</v>
       </c>
       <c r="B36" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C36" s="59"/>
       <c r="D36" s="60" t="str">
@@ -3602,7 +3602,7 @@
         <v>61</v>
       </c>
       <c r="B37" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C37" s="68"/>
       <c r="D37" s="69" t="str">
@@ -3618,7 +3618,7 @@
         <v>50</v>
       </c>
       <c r="B38" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C38" s="59"/>
       <c r="D38" s="60" t="str">
@@ -3634,7 +3634,7 @@
         <v>51</v>
       </c>
       <c r="B39" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C39" s="59"/>
       <c r="D39" s="60" t="str">
@@ -3650,7 +3650,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C40" s="59"/>
       <c r="D40" s="60" t="str">
@@ -3666,7 +3666,7 @@
         <v>55</v>
       </c>
       <c r="B41" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C41" s="59"/>
       <c r="D41" s="60" t="str">
@@ -3682,7 +3682,7 @@
         <v>6</v>
       </c>
       <c r="B42" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C42" s="59"/>
       <c r="D42" s="60" t="str">
@@ -3698,7 +3698,7 @@
         <v>34</v>
       </c>
       <c r="B43" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C43" s="68"/>
       <c r="D43" s="69" t="str">
@@ -3714,7 +3714,7 @@
         <v>35</v>
       </c>
       <c r="B44" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C44" s="59"/>
       <c r="D44" s="60" t="str">
@@ -3730,7 +3730,7 @@
         <v>36</v>
       </c>
       <c r="B45" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C45" s="59"/>
       <c r="D45" s="60" t="str">
@@ -3746,7 +3746,7 @@
         <v>27</v>
       </c>
       <c r="B46" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="59"/>
       <c r="D46" s="60" t="str">
@@ -3762,7 +3762,7 @@
         <v>28</v>
       </c>
       <c r="B47" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C47" s="59"/>
       <c r="D47" s="60" t="str">
@@ -3778,7 +3778,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C48" s="59"/>
       <c r="D48" s="60" t="str">
@@ -3794,7 +3794,7 @@
         <v>45</v>
       </c>
       <c r="B49" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C49" s="59"/>
       <c r="D49" s="60" t="str">
@@ -3810,7 +3810,7 @@
         <v>40</v>
       </c>
       <c r="B50" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C50" s="59"/>
       <c r="D50" s="60" t="str">
@@ -3826,7 +3826,7 @@
         <v>29</v>
       </c>
       <c r="B51" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C51" s="59"/>
       <c r="D51" s="60" t="str">
@@ -3842,7 +3842,7 @@
         <v>24</v>
       </c>
       <c r="B52" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C52" s="59"/>
       <c r="D52" s="60" t="str">
@@ -3858,7 +3858,7 @@
         <v>46</v>
       </c>
       <c r="B53" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C53" s="59"/>
       <c r="D53" s="60" t="str">
@@ -3874,7 +3874,7 @@
         <v>42</v>
       </c>
       <c r="B54" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C54" s="59"/>
       <c r="D54" s="60" t="str">
@@ -3890,7 +3890,7 @@
         <v>38</v>
       </c>
       <c r="B55" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C55" s="59"/>
       <c r="D55" s="60" t="str">
@@ -3906,7 +3906,7 @@
         <v>25</v>
       </c>
       <c r="B56" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C56" s="59"/>
       <c r="D56" s="60" t="str">
@@ -3922,7 +3922,7 @@
         <v>47</v>
       </c>
       <c r="B57" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C57" s="59"/>
       <c r="D57" s="60" t="str">
@@ -3938,7 +3938,7 @@
         <v>43</v>
       </c>
       <c r="B58" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C58" s="59"/>
       <c r="D58" s="60" t="str">
@@ -3954,7 +3954,7 @@
         <v>39</v>
       </c>
       <c r="B59" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C59" s="59"/>
       <c r="D59" s="60" t="str">
@@ -3970,7 +3970,7 @@
         <v>26</v>
       </c>
       <c r="B60" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C60" s="59"/>
       <c r="D60" s="60" t="str">
@@ -3986,7 +3986,7 @@
         <v>49</v>
       </c>
       <c r="B61" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C61" s="59"/>
       <c r="D61" s="60" t="str">
@@ -4002,7 +4002,7 @@
         <v>44</v>
       </c>
       <c r="B62" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C62" s="59"/>
       <c r="D62" s="60" t="str">
@@ -4018,7 +4018,7 @@
         <v>30</v>
       </c>
       <c r="B63" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C63" s="63"/>
       <c r="D63" s="64" t="str">
@@ -4030,21 +4030,30 @@
       <c r="G63"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="114" t="s">
-        <v>140</v>
-      </c>
-      <c r="B64" s="114"/>
-      <c r="C64" s="114"/>
-      <c r="D64" s="114"/>
+      <c r="A64" s="115" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" s="115"/>
+      <c r="C64" s="115"/>
+      <c r="D64" s="115"/>
       <c r="G64"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{4D093F72-1DF5-4965-BD9A-E1DB76A854CB}" showPageBreaks="1" fitToPage="1" printArea="1">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <customSheetView guid="{FF4C21BB-01EC-4FF2-8909-E522D2CCA860}" fitToPage="1" topLeftCell="A14">
+      <selection activeCell="J22" sqref="J22"/>
       <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
       <printOptions horizontalCentered="1" verticalCentered="1"/>
-      <pageSetup paperSize="10" scale="10" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+      <pageSetup paperSize="10" scale="64" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+      <headerFooter alignWithMargins="0">
+        <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
+      </headerFooter>
+    </customSheetView>
+    <customSheetView guid="{3C9A1B9A-18C0-485E-B0F5-D3BF50A001C5}" fitToPage="1" topLeftCell="A22">
+      <selection activeCell="K59" sqref="K59"/>
+      <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
+      <printOptions horizontalCentered="1" verticalCentered="1"/>
+      <pageSetup paperSize="10" scale="61" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
       <headerFooter alignWithMargins="0">
         <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
       </headerFooter>
@@ -4053,25 +4062,16 @@
       <selection activeCell="K59" sqref="K59"/>
       <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
       <printOptions horizontalCentered="1" verticalCentered="1"/>
-      <pageSetup paperSize="10" scale="61" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
-      <headerFooter alignWithMargins="0">
-        <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
-      </headerFooter>
-    </customSheetView>
-    <customSheetView guid="{3C9A1B9A-18C0-485E-B0F5-D3BF50A001C5}" fitToPage="1" topLeftCell="A22">
-      <selection activeCell="K59" sqref="K59"/>
-      <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
-      <printOptions horizontalCentered="1" verticalCentered="1"/>
       <pageSetup paperSize="10" scale="61" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId3"/>
       <headerFooter alignWithMargins="0">
         <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{FF4C21BB-01EC-4FF2-8909-E522D2CCA860}" fitToPage="1" topLeftCell="A14">
-      <selection activeCell="J22" sqref="J22"/>
+    <customSheetView guid="{4D093F72-1DF5-4965-BD9A-E1DB76A854CB}" showPageBreaks="1" fitToPage="1" printArea="1">
+      <selection activeCell="Q21" sqref="Q21"/>
       <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
       <printOptions horizontalCentered="1" verticalCentered="1"/>
-      <pageSetup paperSize="10" scale="64" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId4"/>
+      <pageSetup paperSize="10" scale="10" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId4"/>
       <headerFooter alignWithMargins="0">
         <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
       </headerFooter>
@@ -4152,7 +4152,7 @@
         <v>66</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>78</v>
@@ -4169,7 +4169,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="55"/>
       <c r="D4" s="73" t="str">
@@ -4184,7 +4184,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="60" t="str">
@@ -4199,7 +4199,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="60" t="str">
@@ -4214,7 +4214,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="60" t="str">
@@ -4226,10 +4226,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="60" t="str">
@@ -4244,7 +4244,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="59"/>
       <c r="D9" s="60" t="str">
@@ -4259,7 +4259,7 @@
         <v>41</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="60" t="str">
@@ -4274,7 +4274,7 @@
         <v>65</v>
       </c>
       <c r="B11" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="60" t="str">
@@ -4289,7 +4289,7 @@
         <v>53</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="60" t="str">
@@ -4304,7 +4304,7 @@
         <v>52</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="60" t="str">
@@ -4319,7 +4319,7 @@
         <v>54</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="60" t="str">
@@ -4334,7 +4334,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="60" t="str">
@@ -4349,7 +4349,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C16" s="59"/>
       <c r="D16" s="60" t="str">
@@ -4364,7 +4364,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="60" t="str">
@@ -4379,7 +4379,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="60" t="str">
@@ -4394,7 +4394,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" s="59"/>
       <c r="D19" s="60" t="str">
@@ -4409,7 +4409,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" s="59"/>
       <c r="D20" s="60" t="str">
@@ -4424,7 +4424,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="60" t="str">
@@ -4439,7 +4439,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="59"/>
       <c r="D22" s="60" t="str">
@@ -4454,7 +4454,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C23" s="59"/>
       <c r="D23" s="60" t="str">
@@ -4469,7 +4469,7 @@
         <v>63</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C24" s="59"/>
       <c r="D24" s="60" t="str">
@@ -4484,7 +4484,7 @@
         <v>64</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C25" s="59"/>
       <c r="D25" s="60" t="str">
@@ -4499,7 +4499,7 @@
         <v>61</v>
       </c>
       <c r="B26" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="59"/>
       <c r="D26" s="60" t="str">
@@ -4514,7 +4514,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C27" s="59"/>
       <c r="D27" s="60" t="str">
@@ -4529,7 +4529,7 @@
         <v>51</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C28" s="59"/>
       <c r="D28" s="60" t="str">
@@ -4544,7 +4544,7 @@
         <v>56</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" s="59"/>
       <c r="D29" s="60" t="str">
@@ -4559,7 +4559,7 @@
         <v>55</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C30" s="59"/>
       <c r="D30" s="60" t="str">
@@ -4574,7 +4574,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C31" s="59"/>
       <c r="D31" s="60" t="str">
@@ -4589,7 +4589,7 @@
         <v>34</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C32" s="68"/>
       <c r="D32" s="69" t="str">
@@ -4604,7 +4604,7 @@
         <v>35</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C33" s="59"/>
       <c r="D33" s="60" t="str">
@@ -4619,7 +4619,7 @@
         <v>36</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C34" s="59"/>
       <c r="D34" s="60" t="str">
@@ -4634,7 +4634,7 @@
         <v>48</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" s="59"/>
       <c r="D35" s="60" t="str">
@@ -4649,7 +4649,7 @@
         <v>45</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C36" s="59"/>
       <c r="D36" s="60" t="str">
@@ -4664,7 +4664,7 @@
         <v>40</v>
       </c>
       <c r="B37" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C37" s="59"/>
       <c r="D37" s="60" t="str">
@@ -4679,7 +4679,7 @@
         <v>24</v>
       </c>
       <c r="B38" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C38" s="59"/>
       <c r="D38" s="60" t="str">
@@ -4694,7 +4694,7 @@
         <v>46</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C39" s="59"/>
       <c r="D39" s="60" t="str">
@@ -4709,7 +4709,7 @@
         <v>42</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C40" s="59"/>
       <c r="D40" s="60" t="str">
@@ -4724,7 +4724,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C41" s="59"/>
       <c r="D41" s="60" t="str">
@@ -4739,7 +4739,7 @@
         <v>25</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C42" s="59"/>
       <c r="D42" s="60" t="str">
@@ -4754,7 +4754,7 @@
         <v>47</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C43" s="59"/>
       <c r="D43" s="60" t="str">
@@ -4769,7 +4769,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C44" s="59"/>
       <c r="D44" s="60" t="str">
@@ -4784,7 +4784,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C45" s="59"/>
       <c r="D45" s="60" t="str">
@@ -4799,7 +4799,7 @@
         <v>49</v>
       </c>
       <c r="B46" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="59"/>
       <c r="D46" s="60" t="str">
@@ -4814,7 +4814,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="70" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C47" s="63"/>
       <c r="D47" s="64" t="str">
@@ -4825,12 +4825,12 @@
       <c r="F47"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="114" t="s">
-        <v>140</v>
-      </c>
-      <c r="B48" s="114"/>
-      <c r="C48" s="114"/>
-      <c r="D48" s="114"/>
+      <c r="A48" s="115" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="115"/>
+      <c r="C48" s="115"/>
+      <c r="D48" s="115"/>
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E49" s="9"/>
@@ -4842,11 +4842,20 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{4D093F72-1DF5-4965-BD9A-E1DB76A854CB}" showPageBreaks="1" fitToPage="1" printArea="1" topLeftCell="C1">
-      <selection activeCell="L3" sqref="L3"/>
+    <customSheetView guid="{FF4C21BB-01EC-4FF2-8909-E522D2CCA860}" fitToPage="1">
+      <selection activeCell="V39" sqref="V39"/>
       <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
       <printOptions horizontalCentered="1" verticalCentered="1"/>
-      <pageSetup paperSize="10" scale="10" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+      <pageSetup paperSize="10" scale="71" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+      <headerFooter alignWithMargins="0">
+        <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
+      </headerFooter>
+    </customSheetView>
+    <customSheetView guid="{3C9A1B9A-18C0-485E-B0F5-D3BF50A001C5}" fitToPage="1">
+      <selection activeCell="A46" sqref="A46:K46"/>
+      <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
+      <printOptions horizontalCentered="1" verticalCentered="1"/>
+      <pageSetup paperSize="10" scale="70" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
       <headerFooter alignWithMargins="0">
         <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
       </headerFooter>
@@ -4855,25 +4864,16 @@
       <selection activeCell="A46" sqref="A46:K46"/>
       <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
       <printOptions horizontalCentered="1" verticalCentered="1"/>
-      <pageSetup paperSize="10" scale="70" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
-      <headerFooter alignWithMargins="0">
-        <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
-      </headerFooter>
-    </customSheetView>
-    <customSheetView guid="{3C9A1B9A-18C0-485E-B0F5-D3BF50A001C5}" fitToPage="1">
-      <selection activeCell="A46" sqref="A46:K46"/>
-      <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
-      <printOptions horizontalCentered="1" verticalCentered="1"/>
       <pageSetup paperSize="10" scale="70" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId3"/>
       <headerFooter alignWithMargins="0">
         <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{FF4C21BB-01EC-4FF2-8909-E522D2CCA860}" fitToPage="1">
-      <selection activeCell="V39" sqref="V39"/>
+    <customSheetView guid="{4D093F72-1DF5-4965-BD9A-E1DB76A854CB}" showPageBreaks="1" fitToPage="1" printArea="1" topLeftCell="C1">
+      <selection activeCell="L3" sqref="L3"/>
       <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
       <printOptions horizontalCentered="1" verticalCentered="1"/>
-      <pageSetup paperSize="10" scale="71" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId4"/>
+      <pageSetup paperSize="10" scale="10" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId4"/>
       <headerFooter alignWithMargins="0">
         <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
       </headerFooter>
@@ -4949,7 +4949,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>78</v>
@@ -4964,7 +4964,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="55"/>
       <c r="D4" s="56" t="str">
@@ -4979,7 +4979,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="60" t="str">
@@ -4994,7 +4994,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="60" t="str">
@@ -5009,7 +5009,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="60" t="str">
@@ -5021,10 +5021,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="60" t="str">
@@ -5039,7 +5039,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="59"/>
       <c r="D9" s="60" t="str">
@@ -5054,7 +5054,7 @@
         <v>41</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="60" t="str">
@@ -5069,7 +5069,7 @@
         <v>65</v>
       </c>
       <c r="B11" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="60" t="str">
@@ -5084,7 +5084,7 @@
         <v>53</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="60" t="str">
@@ -5099,7 +5099,7 @@
         <v>52</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="60" t="str">
@@ -5114,7 +5114,7 @@
         <v>54</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="60" t="str">
@@ -5129,7 +5129,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="60" t="str">
@@ -5144,7 +5144,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C16" s="59"/>
       <c r="D16" s="60" t="str">
@@ -5159,7 +5159,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="60" t="str">
@@ -5174,7 +5174,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="60" t="str">
@@ -5189,7 +5189,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" s="59"/>
       <c r="D19" s="60" t="str">
@@ -5204,7 +5204,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" s="59"/>
       <c r="D20" s="60" t="str">
@@ -5219,7 +5219,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="60" t="str">
@@ -5234,7 +5234,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="59"/>
       <c r="D22" s="60" t="str">
@@ -5249,7 +5249,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C23" s="59"/>
       <c r="D23" s="60" t="str">
@@ -5264,7 +5264,7 @@
         <v>63</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C24" s="59"/>
       <c r="D24" s="60" t="str">
@@ -5279,7 +5279,7 @@
         <v>64</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C25" s="59"/>
       <c r="D25" s="60" t="str">
@@ -5294,7 +5294,7 @@
         <v>61</v>
       </c>
       <c r="B26" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="59"/>
       <c r="D26" s="60" t="str">
@@ -5309,7 +5309,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C27" s="59"/>
       <c r="D27" s="60" t="str">
@@ -5324,7 +5324,7 @@
         <v>51</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C28" s="59"/>
       <c r="D28" s="60" t="str">
@@ -5339,7 +5339,7 @@
         <v>56</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" s="59"/>
       <c r="D29" s="60" t="str">
@@ -5354,7 +5354,7 @@
         <v>55</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C30" s="59"/>
       <c r="D30" s="60" t="str">
@@ -5369,7 +5369,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C31" s="59"/>
       <c r="D31" s="60" t="str">
@@ -5384,7 +5384,7 @@
         <v>34</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C32" s="68"/>
       <c r="D32" s="69" t="str">
@@ -5399,7 +5399,7 @@
         <v>35</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C33" s="59"/>
       <c r="D33" s="60" t="str">
@@ -5414,7 +5414,7 @@
         <v>36</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C34" s="59"/>
       <c r="D34" s="60" t="str">
@@ -5429,7 +5429,7 @@
         <v>48</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" s="59"/>
       <c r="D35" s="60" t="str">
@@ -5444,7 +5444,7 @@
         <v>45</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C36" s="59"/>
       <c r="D36" s="60" t="str">
@@ -5459,7 +5459,7 @@
         <v>40</v>
       </c>
       <c r="B37" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C37" s="59"/>
       <c r="D37" s="60" t="str">
@@ -5474,7 +5474,7 @@
         <v>24</v>
       </c>
       <c r="B38" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C38" s="59"/>
       <c r="D38" s="60" t="str">
@@ -5489,7 +5489,7 @@
         <v>46</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C39" s="59"/>
       <c r="D39" s="60" t="str">
@@ -5504,7 +5504,7 @@
         <v>42</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C40" s="59"/>
       <c r="D40" s="60" t="str">
@@ -5519,7 +5519,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C41" s="59"/>
       <c r="D41" s="60" t="str">
@@ -5534,7 +5534,7 @@
         <v>25</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C42" s="59"/>
       <c r="D42" s="60" t="str">
@@ -5549,7 +5549,7 @@
         <v>47</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C43" s="59"/>
       <c r="D43" s="60" t="str">
@@ -5564,7 +5564,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C44" s="59"/>
       <c r="D44" s="60" t="str">
@@ -5579,7 +5579,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C45" s="59"/>
       <c r="D45" s="60" t="str">
@@ -5594,7 +5594,7 @@
         <v>49</v>
       </c>
       <c r="B46" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="59"/>
       <c r="D46" s="60" t="str">
@@ -5609,7 +5609,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="70" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C47" s="63"/>
       <c r="D47" s="64" t="str">
@@ -5620,12 +5620,12 @@
       <c r="F47"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="114" t="s">
-        <v>140</v>
-      </c>
-      <c r="B48" s="114"/>
-      <c r="C48" s="114"/>
-      <c r="D48" s="114"/>
+      <c r="A48" s="115" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="115"/>
+      <c r="C48" s="115"/>
+      <c r="D48" s="115"/>
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E49" s="9"/>
@@ -5641,11 +5641,20 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{4D093F72-1DF5-4965-BD9A-E1DB76A854CB}" showPageBreaks="1" fitToPage="1" printArea="1" topLeftCell="C1">
-      <selection activeCell="L3" sqref="L3"/>
+    <customSheetView guid="{FF4C21BB-01EC-4FF2-8909-E522D2CCA860}" fitToPage="1">
+      <selection activeCell="J45" sqref="J45"/>
       <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
       <printOptions horizontalCentered="1" verticalCentered="1"/>
-      <pageSetup paperSize="10" scale="10" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+      <pageSetup paperSize="10" scale="71" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+      <headerFooter alignWithMargins="0">
+        <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
+      </headerFooter>
+    </customSheetView>
+    <customSheetView guid="{3C9A1B9A-18C0-485E-B0F5-D3BF50A001C5}" fitToPage="1" topLeftCell="A7">
+      <selection activeCell="F47" sqref="F47"/>
+      <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
+      <printOptions horizontalCentered="1" verticalCentered="1"/>
+      <pageSetup paperSize="10" scale="70" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
       <headerFooter alignWithMargins="0">
         <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
       </headerFooter>
@@ -5654,25 +5663,16 @@
       <selection activeCell="F47" sqref="F47"/>
       <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
       <printOptions horizontalCentered="1" verticalCentered="1"/>
-      <pageSetup paperSize="10" scale="70" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
-      <headerFooter alignWithMargins="0">
-        <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
-      </headerFooter>
-    </customSheetView>
-    <customSheetView guid="{3C9A1B9A-18C0-485E-B0F5-D3BF50A001C5}" fitToPage="1" topLeftCell="A7">
-      <selection activeCell="F47" sqref="F47"/>
-      <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
-      <printOptions horizontalCentered="1" verticalCentered="1"/>
       <pageSetup paperSize="10" scale="70" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId3"/>
       <headerFooter alignWithMargins="0">
         <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{FF4C21BB-01EC-4FF2-8909-E522D2CCA860}" fitToPage="1">
-      <selection activeCell="J45" sqref="J45"/>
+    <customSheetView guid="{4D093F72-1DF5-4965-BD9A-E1DB76A854CB}" showPageBreaks="1" fitToPage="1" printArea="1" topLeftCell="C1">
+      <selection activeCell="L3" sqref="L3"/>
       <pageMargins left="0.31" right="0.31" top="0.31" bottom="0.31" header="0.31" footer="0.39000000000000007"/>
       <printOptions horizontalCentered="1" verticalCentered="1"/>
-      <pageSetup paperSize="10" scale="71" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId4"/>
+      <pageSetup paperSize="10" scale="10" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId4"/>
       <headerFooter alignWithMargins="0">
         <oddFooter>&amp;L&amp;F&amp;Rpage &amp;P/&amp;N</oddFooter>
       </headerFooter>
@@ -5743,7 +5743,7 @@
         <v>66</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>78</v>
@@ -5759,7 +5759,7 @@
         <v>67</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="55"/>
       <c r="D4" s="56" t="str">
@@ -5774,7 +5774,7 @@
         <v>71</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="60" t="str">
@@ -5789,7 +5789,7 @@
         <v>68</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="60" t="str">
@@ -5804,7 +5804,7 @@
         <v>72</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="60" t="str">
@@ -5819,7 +5819,7 @@
         <v>70</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="60" t="str">
@@ -5834,7 +5834,7 @@
         <v>69</v>
       </c>
       <c r="B9" s="62" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="63"/>
       <c r="D9" s="64" t="str">

</xml_diff>